<commit_message>
Added in Fleet 6 and 7 index tables
</commit_message>
<xml_diff>
--- a/txt_files/Fleet6and7_OnboardObserver_IndexData.xlsx
+++ b/txt_files/Fleet6and7_OnboardObserver_IndexData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11777" windowHeight="4483" tabRatio="789" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11777" windowHeight="4483" tabRatio="789"/>
   </bookViews>
   <sheets>
     <sheet name="NorthAIC" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Model</t>
   </si>
@@ -104,9 +104,6 @@
     <t>\textbf{13921}</t>
   </si>
   <si>
-    <t>\extbf{16674}</t>
-  </si>
-  <si>
     <t>Filter to drifts within 43 m of a reef,97% quantile</t>
   </si>
   <si>
@@ -135,6 +132,12 @@
   </si>
   <si>
     <t>Filter to drifts with &gt;=20% groundfish and recheck reefs</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>\textbf{16674}</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -553,7 +556,7 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -628,18 +631,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
         <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>2663</v>
@@ -657,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -778,9 +781,20 @@
         <v>7250</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2">
         <v>13792</v>
@@ -791,7 +805,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2">
         <v>13145</v>
@@ -802,7 +816,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2">
         <v>12965</v>
@@ -811,9 +825,20 @@
         <v>5796</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
         <v>11635</v>
@@ -824,7 +849,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2">
         <v>5495</v>
@@ -835,7 +860,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2">
         <v>5440</v>
@@ -872,7 +897,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2">
         <v>13792</v>
@@ -883,7 +908,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2">
         <v>13145</v>
@@ -894,7 +919,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>12965</v>
@@ -931,7 +956,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2">
         <v>11635</v>
@@ -942,7 +967,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2">
         <v>5495</v>
@@ -953,7 +978,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>5440</v>

</xml_diff>

<commit_message>
Fixed table error Fleet6_7_Filter
</commit_message>
<xml_diff>
--- a/txt_files/Fleet6and7_OnboardObserver_IndexData.xlsx
+++ b/txt_files/Fleet6and7_OnboardObserver_IndexData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11777" windowHeight="4483" tabRatio="789"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11777" windowHeight="4483" tabRatio="789" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NorthAIC" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>Model</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>\textbf{16674}</t>
+  </si>
+  <si>
+    <t>Filter to drifts within 43 m of a reef, 97% quantile</t>
   </si>
 </sst>
 </file>
@@ -476,7 +479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -660,13 +663,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.765625" customWidth="1"/>
+    <col min="1" max="1" width="48.765625" customWidth="1"/>
     <col min="2" max="2" width="18.3046875" customWidth="1"/>
     <col min="3" max="3" width="20.921875" customWidth="1"/>
   </cols>
@@ -805,7 +808,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B13" s="2">
         <v>13145</v>

</xml_diff>